<commit_message>
Leves modificaciones al codigo fuente
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -342,7 +342,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -398,6 +398,38 @@
         <v>43878.61451014101</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3006.67</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>43879.75540255231</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3006.67</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>43879.75543708817</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3006.67</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>43879.75547123926</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>3006.67</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>43879.75550549213</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>

</xml_diff>